<commit_message>
Update scraper with new data
</commit_message>
<xml_diff>
--- a/raw_data/earnings.xlsx
+++ b/raw_data/earnings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\dol-smb\dol_shared\DOL0A1FS2\rscommon\Brown, James\Press Release\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0256758-D2C0-4BF7-8445-DF7236C86492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F7CE4D-BC97-4881-920B-4E8C1761E663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="675" yWindow="345" windowWidth="19185" windowHeight="10275" tabRatio="664" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="18045" windowHeight="10335" tabRatio="664" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="average hourly earnings" sheetId="2" r:id="rId1"/>
@@ -323,12 +323,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -338,6 +332,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -689,7 +689,7 @@
   <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+      <selection activeCell="M42" sqref="M42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -699,120 +699,120 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
       <c r="K3" s="23"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
     </row>
     <row r="6" spans="1:14" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
     </row>
     <row r="7" spans="1:14" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
     </row>
     <row r="8" spans="1:14" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
     </row>
     <row r="9" spans="1:14" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
     </row>
     <row r="12" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1600,9 +1600,11 @@
         <v>41.5</v>
       </c>
       <c r="J29" s="7">
-        <v>41.57</v>
-      </c>
-      <c r="K29" s="7"/>
+        <v>41.66</v>
+      </c>
+      <c r="K29" s="7">
+        <v>42</v>
+      </c>
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
       <c r="N29" s="12"/>
@@ -2161,25 +2163,28 @@
       </c>
       <c r="J40" s="10">
         <f t="shared" si="9"/>
-        <v>3.3791938209026817E-3</v>
-      </c>
-      <c r="K40" s="10"/>
+        <v>5.5515327057686914E-3</v>
+      </c>
+      <c r="K40" s="10">
+        <f t="shared" si="9"/>
+        <v>-8.0302314596127911E-3</v>
+      </c>
       <c r="L40" s="10"/>
       <c r="M40" s="10"/>
       <c r="N40" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B6:G6"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="A5:F5"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B6:G6"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2195,7 +2200,7 @@
   <dimension ref="A1:N41"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2205,54 +2210,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
@@ -2261,10 +2266,10 @@
       <c r="B6" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
@@ -2273,10 +2278,10 @@
       <c r="B7" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
@@ -2285,10 +2290,10 @@
       <c r="B8" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
@@ -2297,10 +2302,10 @@
       <c r="B9" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
@@ -2309,10 +2314,10 @@
       <c r="B10" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
@@ -2321,10 +2326,10 @@
       <c r="B11" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
@@ -3107,9 +3112,11 @@
         <v>32.4</v>
       </c>
       <c r="J30" s="19">
-        <v>32.299999999999997</v>
-      </c>
-      <c r="K30" s="19"/>
+        <v>32.200000000000003</v>
+      </c>
+      <c r="K30" s="19">
+        <v>32.9</v>
+      </c>
       <c r="L30" s="19"/>
       <c r="M30" s="19"/>
       <c r="N30" s="19"/>
@@ -3681,9 +3688,12 @@
       </c>
       <c r="J41" s="10">
         <f t="shared" si="9"/>
-        <v>-3.0030030030030019E-2</v>
-      </c>
-      <c r="K41" s="10"/>
+        <v>-3.3033033033032844E-2</v>
+      </c>
+      <c r="K41" s="10">
+        <f t="shared" si="9"/>
+        <v>-2.3738872403560984E-2</v>
+      </c>
       <c r="L41" s="10"/>
       <c r="M41" s="10"/>
       <c r="N41" s="14"/>
@@ -3716,7 +3726,7 @@
   <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3727,114 +3737,114 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
@@ -3843,10 +3853,10 @@
       <c r="B11" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
     </row>
     <row r="13" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -4629,9 +4639,11 @@
         <v>1344.6</v>
       </c>
       <c r="J30" s="11">
-        <v>1342.71</v>
-      </c>
-      <c r="K30" s="11"/>
+        <v>1341.45</v>
+      </c>
+      <c r="K30" s="11">
+        <v>1381.8</v>
+      </c>
       <c r="L30" s="11"/>
       <c r="M30" s="11"/>
       <c r="N30" s="16"/>
@@ -5146,22 +5158,26 @@
       </c>
       <c r="J40" s="10">
         <f t="shared" si="7"/>
-        <v>-2.6753743784520223E-2</v>
+        <v>-2.7667038749800588E-2</v>
+      </c>
+      <c r="K40" s="10">
+        <f t="shared" si="7"/>
+        <v>-3.1579832639502037E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="A5:F5"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="B7:F7"/>
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="B9:F9"/>
     <mergeCell ref="B10:F10"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="A5:F5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>